<commit_message>
reorg & remove ugly output
</commit_message>
<xml_diff>
--- a/Baselining/ML algo compare data.xlsx
+++ b/Baselining/ML algo compare data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\ok-boomer\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kali\Documents\GitHub\CMPT-419\Baselining\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E730B60D-177D-4C84-AB74-122DEB1DEBA4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2034357D-1217-4857-8C68-C3AE471F16C0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3075" windowWidth="28800" windowHeight="11385" xr2:uid="{EC025888-F4B1-4839-9169-F334C0243451}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{EC025888-F4B1-4839-9169-F334C0243451}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -66,7 +66,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -76,21 +76,9 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFD5D5D5"/>
-      <name val="Courier New"/>
-      <family val="3"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFCE9178"/>
-      <name val="Courier New"/>
-      <family val="3"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF6AA94F"/>
-      <name val="Courier New"/>
-      <family val="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -113,13 +101,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1570,7 +1555,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1587,91 +1572,79 @@
       <c r="B1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="1">
-        <v>13.218540750172901</v>
-      </c>
+      <c r="C1" s="1"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="A2" s="1">
         <v>12.462999999999999</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2">
-        <v>12.4631028013175</v>
-      </c>
+      <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="A3" s="1">
         <v>17.856999999999999</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C3">
-        <v>17.856727259041001</v>
-      </c>
+      <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="A4" s="1">
         <v>12.475</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C4">
-        <v>12.4749147165031</v>
-      </c>
+      <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>14.87</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="1">
-        <v>14.8715592462811</v>
-      </c>
+      <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
+      <c r="A6" s="2">
         <v>14.63</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="C6" s="1"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
+      <c r="A7" s="2">
         <v>16.600000000000001</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="C7" s="1"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8">
+      <c r="A8" s="1">
         <v>15.127000000000001</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C8">
-        <v>15.1265618293949</v>
-      </c>
+      <c r="C8" s="1"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9">
+      <c r="A9" s="1">
         <v>17.856999999999999</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C9">
-        <v>17.856727259041001</v>
-      </c>
+      <c r="C9" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>